<commit_message>
_ Updated version of the Industry_model_final.py   * All issues were solved   * Emissions optimization is now possible _ 2015 steel industry case study that can be found here: https://www.overleaf.com/read/chsvfsqsncjf
</commit_message>
<xml_diff>
--- a/Models/Industry_model/Input/Steel/Data/v2/Resources_Technologies.xlsx
+++ b/Models/Industry_model/Input/Steel/Data/v2/Resources_Technologies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q.raillard-cazanove\ownCloud\1ère année\Optim modelling\Project\Etude_TP_CapaExpPlaning-Python\Models\Industry_model\Input\Steel\Data\v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34E64C2-F198-4E43-8A52-7A17F09DBCFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D978EDE9-558C-4184-872E-1CE5FDAE3D1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1227,7 +1227,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>